<commit_message>
Need to pull the flickr data down, parse it, and then pull the photo
</commit_message>
<xml_diff>
--- a/photolist.xlsx
+++ b/photolist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaron/Documents/Python Code/download_memorybook_photos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1887F08-CBEC-3E45-8A70-AA24870B3AC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9309A9-15D4-F047-952D-E8857A8522AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10380" yWindow="1920" windowWidth="17340" windowHeight="9580" xr2:uid="{9F72C116-6C8E-0D4A-8BDB-7E4359E9C28C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Team</t>
   </si>
@@ -45,30 +45,6 @@
     <t>JV</t>
   </si>
   <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/45160698381/in/datetaken/</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/45160697281/in/datetaken/</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/44201228544/in/album-72157698526626812/</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/43108996450/in/album-72157698526626812/</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/31048125348/in/album-72157698526626812/</t>
-  </si>
-  <si>
-    <t>Varsity</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/43046152175/in/album-72157698924162004/</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/29013600377/in/album-72157698924162004/</t>
-  </si>
-  <si>
     <t>Player_Name</t>
   </si>
   <si>
@@ -78,28 +54,10 @@
     <t>Photo5</t>
   </si>
   <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/29013598477/in/album-72157698924162004/</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/43903291662/in/album-72157698924162004/</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/45160695761/in/datetaken/</t>
-  </si>
-  <si>
     <t>Tom</t>
   </si>
   <si>
-    <t>Dick</t>
-  </si>
-  <si>
-    <t>Harry</t>
-  </si>
-  <si>
-    <t>Bill</t>
-  </si>
-  <si>
-    <t>https://www.google.com/imgres?imgurl=https%3A%2F%2Fimages.pexels.com%2Fphotos%2F46710%2Fpexels-photo-46710.jpeg%3Fauto%3Dcompress%26cs%3Dtinysrgb%26h%3D350&amp;imgrefurl=https%3A%2F%2Fwww.pexels.com%2Fsearch%2Fsummer%2F&amp;docid=MLbH2w6jfwuHxM&amp;tbnid=jN-Br1KRhWXbhM%3A&amp;vet=10ahUKEwih_KHyxP3dAhVDi1kKHUn0CbIQMwh9KAEwAQ..i&amp;w=525&amp;h=350&amp;bih=888&amp;biw=1405&amp;q=photos&amp;ved=0ahUKEwih_KHyxP3dAhVDi1kKHUn0CbIQMwh9KAEwAQ&amp;iact=mrc&amp;uact=8</t>
+    <t>https://www.flickr.com/photos/jakubz/30287928287/in/feed</t>
   </si>
 </sst>
 </file>
@@ -462,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4A9BFD-7491-0849-B5A9-9AC4ABF4E2DD}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,7 +440,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -497,10 +455,10 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -508,87 +466,20 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>24</v>
-      </c>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{EB841AF9-6B4D-464C-A522-8824E1DE2F00}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{94BB15EB-2CE3-0F47-9B0C-035DEE8DE8CF}"/>
-    <hyperlink ref="D2" r:id="rId3" xr:uid="{B84CFE1E-CBBC-C647-8490-7F52254AD6F7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added in the flickr api call to getsizes and actually download the photos.
</commit_message>
<xml_diff>
--- a/photolist.xlsx
+++ b/photolist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaron/Documents/Python Code/download_memorybook_photos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9309A9-15D4-F047-952D-E8857A8522AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438E056B-FE59-F144-91CF-D5A9BA315AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10380" yWindow="1920" windowWidth="17340" windowHeight="9580" xr2:uid="{9F72C116-6C8E-0D4A-8BDB-7E4359E9C28C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Team</t>
   </si>
@@ -45,6 +45,12 @@
     <t>JV</t>
   </si>
   <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/45160698381/in/datetaken/</t>
+  </si>
+  <si>
+    <t>Varsity</t>
+  </si>
+  <si>
     <t>Player_Name</t>
   </si>
   <si>
@@ -57,14 +63,26 @@
     <t>Tom</t>
   </si>
   <si>
-    <t>https://www.flickr.com/photos/jakubz/30287928287/in/feed</t>
+    <t>Dick</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Smoosh</t>
+  </si>
+  <si>
+    <t>Rebels</t>
+  </si>
+  <si>
+    <t>Alex</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,6 +94,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -102,9 +128,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4A9BFD-7491-0849-B5A9-9AC4ABF4E2DD}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -435,12 +462,12 @@
     <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -455,29 +482,120 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
-        <v>8</v>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D3" s="1"/>
-      <c r="F3" s="1"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added password.py for passwords
</commit_message>
<xml_diff>
--- a/photolist.xlsx
+++ b/photolist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaron/Documents/Python Code/download_memorybook_photos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438E056B-FE59-F144-91CF-D5A9BA315AC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CCF070-D2DA-0243-8426-4EB4AB226B7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10380" yWindow="1920" windowWidth="17340" windowHeight="9580" xr2:uid="{9F72C116-6C8E-0D4A-8BDB-7E4359E9C28C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t>Team</t>
   </si>
@@ -45,12 +45,6 @@
     <t>JV</t>
   </si>
   <si>
-    <t>https://www.flickr.com/photos/aaronhatcher/45160698381/in/datetaken/</t>
-  </si>
-  <si>
-    <t>Varsity</t>
-  </si>
-  <si>
     <t>Player_Name</t>
   </si>
   <si>
@@ -60,29 +54,50 @@
     <t>Photo5</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Dick</t>
-  </si>
-  <si>
-    <t>Harry</t>
-  </si>
-  <si>
-    <t>Smoosh</t>
+    <t>Photo6</t>
+  </si>
+  <si>
+    <t>Photo7</t>
+  </si>
+  <si>
+    <t>Photo8</t>
+  </si>
+  <si>
+    <t>Photo9</t>
+  </si>
+  <si>
+    <t>Photo10</t>
+  </si>
+  <si>
+    <t>Drew Barklay</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44303421911/in/album-72157699031593671/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/43597297365/in/album-72157700729583704/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/29728327737/in/album-72157673392276678/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44666348631/in/album-72157673392276678/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/29623981907/in/album-72157673213389378/</t>
   </si>
   <si>
     <t>Rebels</t>
   </si>
   <si>
-    <t>Alex</t>
+    <t>Adam Hatcher</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,6 +121,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,10 +155,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -447,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4A9BFD-7491-0849-B5A9-9AC4ABF4E2DD}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,12 +491,12 @@
     <col min="6" max="6" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -482,122 +511,112 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2">
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3">
-        <v>19</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>6</v>
-      </c>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>6</v>
-      </c>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>6</v>
-      </c>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{5836B73A-EC68-5945-A693-5F765EF5EC5C}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{79943173-808E-084C-896E-A57963477881}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{9ABB9A47-B6ED-2047-845F-569CE467DB34}"/>
+    <hyperlink ref="G2" r:id="rId4" xr:uid="{4241DB40-081C-D342-8D3E-B6DBDEEEB64E}"/>
+    <hyperlink ref="H2" r:id="rId5" xr:uid="{B08FA963-1AD5-C342-A7ED-6D329D6C43F8}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{CE1B553D-FBA5-634F-84E8-3ED69885C975}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{CDCC40CF-7676-DD49-A918-FBCAE0489D5E}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{E72CD69B-0E1C-044F-825E-DE4FAF9029F1}"/>
+    <hyperlink ref="G3" r:id="rId9" xr:uid="{B522A735-88CB-9749-BA55-B4795F658C91}"/>
+    <hyperlink ref="H3" r:id="rId10" xr:uid="{D36327CB-D66D-F941-9BEE-CC5D8B97FB17}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added functions file and logging
</commit_message>
<xml_diff>
--- a/photolist.xlsx
+++ b/photolist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaron/Documents/Python Code/download_memorybook_photos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CCF070-D2DA-0243-8426-4EB4AB226B7B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073A4750-9398-C549-9A7B-7554FFFA3948}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10380" yWindow="1920" windowWidth="17340" windowHeight="9580" xr2:uid="{9F72C116-6C8E-0D4A-8BDB-7E4359E9C28C}"/>
+    <workbookView xWindow="17660" yWindow="1140" windowWidth="17340" windowHeight="9580" xr2:uid="{9F72C116-6C8E-0D4A-8BDB-7E4359E9C28C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Team</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Photo10</t>
   </si>
   <si>
-    <t>Drew Barklay</t>
-  </si>
-  <si>
     <t>https://www.flickr.com/photos/aaronhatcher/44303421911/in/album-72157699031593671/</t>
   </si>
   <si>
@@ -87,10 +84,79 @@
     <t>https://www.flickr.com/photos/aaronhatcher/29623981907/in/album-72157673213389378/</t>
   </si>
   <si>
-    <t>Rebels</t>
-  </si>
-  <si>
-    <t>Adam Hatcher</t>
+    <t>https://www.flickr.com/photos/aaronhatcher/44815854251/in/album-72157695718027700/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44921041101/in/album-72157698526626812/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/29448835647/in/album-72157700819906805/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/43786276754/in/album-72157701022169035/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/29566593047/in/album-72157701022169035/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/42797091140/in/album-72157673289806428/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/43004907950/in/album-72157695718027700/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/30795644808/in/album-72157673392276678/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44790536451/in/album-72157673602834238/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/43004908230/in/album-72157695718027700/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44201224464/in/album-72157698526626812/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/30919246858/in/album-72157673602834238/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44247376301/in/album-72157670524024857/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44255305832/in/album-72157699031593671/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/43397224615/in/album-72157699031593671/</t>
+  </si>
+  <si>
+    <t>https://farm2.staticflickr.com/1978/44346511884_7b1fff907b_o_d.jpg</t>
+  </si>
+  <si>
+    <t>https://farm2.staticflickr.com/1955/31402386198_f262518aea_o_d.jpg</t>
+  </si>
+  <si>
+    <t>https://farm2.staticflickr.com/1866/29624083197_49d03ec9d3_o_d.jpg</t>
+  </si>
+  <si>
+    <t>https://farm2.staticflickr.com/1843/44790455141_6f20a05bbf_o_d.jpg</t>
+  </si>
+  <si>
+    <t>https://farm2.staticflickr.com/1871/30634437668_9603c4f8b5_o_d.jpg</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44666344741/in/album-72157673392276678/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44921048541/in/album-72157698526626812/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44740716672/in/album-72157673602834238/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/30919341708/in/album-72157673602834238/</t>
+  </si>
+  <si>
+    <t>https://www.flickr.com/photos/aaronhatcher/44740799732/in/album-72157673602834238/</t>
   </si>
 </sst>
 </file>
@@ -114,14 +180,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -130,6 +188,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -476,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A4A9BFD-7491-0849-B5A9-9AC4ABF4E2DD}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -533,89 +597,197 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="4">
-        <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="F3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="3">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D4" s="2"/>
-      <c r="E4" s="1"/>
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2">
+        <v>17</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4">
+        <v>6</v>
+      </c>
+      <c r="C7" s="4">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{5836B73A-EC68-5945-A693-5F765EF5EC5C}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{79943173-808E-084C-896E-A57963477881}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{9ABB9A47-B6ED-2047-845F-569CE467DB34}"/>
-    <hyperlink ref="G2" r:id="rId4" xr:uid="{4241DB40-081C-D342-8D3E-B6DBDEEEB64E}"/>
-    <hyperlink ref="H2" r:id="rId5" xr:uid="{B08FA963-1AD5-C342-A7ED-6D329D6C43F8}"/>
-    <hyperlink ref="D3" r:id="rId6" xr:uid="{CE1B553D-FBA5-634F-84E8-3ED69885C975}"/>
-    <hyperlink ref="E3" r:id="rId7" xr:uid="{CDCC40CF-7676-DD49-A918-FBCAE0489D5E}"/>
-    <hyperlink ref="F3" r:id="rId8" xr:uid="{E72CD69B-0E1C-044F-825E-DE4FAF9029F1}"/>
-    <hyperlink ref="G3" r:id="rId9" xr:uid="{B522A735-88CB-9749-BA55-B4795F658C91}"/>
-    <hyperlink ref="H3" r:id="rId10" xr:uid="{D36327CB-D66D-F941-9BEE-CC5D8B97FB17}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{9A2E206D-1487-374A-87F6-4733BE21057B}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{B1B7AA79-56EA-754F-BF41-53B91724C602}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{BCA0411E-31E6-EE4F-86D5-30017063C6AC}"/>
+    <hyperlink ref="G2" r:id="rId4" xr:uid="{CA423C6D-D213-3146-B17F-BB760C8EBBAB}"/>
+    <hyperlink ref="H2" r:id="rId5" xr:uid="{51EF9DA9-EEDB-1345-9FDD-6A9A9004F53D}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{D804F0D7-EA72-D949-A2E6-79AA37AB5A40}"/>
+    <hyperlink ref="E3" r:id="rId7" xr:uid="{71ABD0E2-ABC4-6649-87CF-1F679F2458A6}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{BE2C3526-C972-8E4C-AFFC-AE764487621C}"/>
+    <hyperlink ref="G3" r:id="rId9" xr:uid="{1C3747C6-04D0-474C-B58A-7D13227A5700}"/>
+    <hyperlink ref="H3" r:id="rId10" xr:uid="{6D224345-331C-1A4F-8201-B03BCF7F9DFA}"/>
+    <hyperlink ref="D4" r:id="rId11" xr:uid="{50C40054-A487-E145-9C22-0A73DBAF04E2}"/>
+    <hyperlink ref="E4" r:id="rId12" xr:uid="{D9F994B3-55AF-4041-8A19-7DD9564DD267}"/>
+    <hyperlink ref="F4" r:id="rId13" xr:uid="{853B9C3C-3D01-AC44-BBB7-A7D0D06AABBE}"/>
+    <hyperlink ref="G4" r:id="rId14" xr:uid="{0DEFC546-2C02-154A-ACD4-AC073D986F68}"/>
+    <hyperlink ref="H4" r:id="rId15" xr:uid="{DCE466AF-6F31-D243-9B6C-092343AAA626}"/>
+    <hyperlink ref="D5" r:id="rId16" xr:uid="{A0D6E6C0-DABF-7A48-B60F-8311FCA83528}"/>
+    <hyperlink ref="E5" r:id="rId17" xr:uid="{EF6D24DA-237F-FD49-868D-FAE76544700F}"/>
+    <hyperlink ref="F5" r:id="rId18" xr:uid="{ABC7EB2A-3305-504F-A15C-74C2D34A7493}"/>
+    <hyperlink ref="G5" r:id="rId19" xr:uid="{9061A9BF-0253-2F43-87DF-6F8FF134040F}"/>
+    <hyperlink ref="H5" r:id="rId20" xr:uid="{F4D55F55-90BE-324C-A738-D555AA2CB18E}"/>
+    <hyperlink ref="D6" r:id="rId21" xr:uid="{78B5A160-7C9A-9D41-B8EF-46F433298B9B}"/>
+    <hyperlink ref="E6" r:id="rId22" xr:uid="{37A6D1DE-D4D3-094B-83F8-C5EF0B8098D6}"/>
+    <hyperlink ref="F6" r:id="rId23" xr:uid="{FADAD4C8-667C-274F-A364-38FC18B8DEA8}"/>
+    <hyperlink ref="G6" r:id="rId24" xr:uid="{CA0503B2-BF7A-0E45-ABC6-4359379EE870}"/>
+    <hyperlink ref="H6" r:id="rId25" xr:uid="{A59CBDEF-6445-9545-A511-6B7F0AB50B83}"/>
+    <hyperlink ref="D7" r:id="rId26" xr:uid="{5672B81B-145B-7649-AF93-8967534223F2}"/>
+    <hyperlink ref="E7" r:id="rId27" xr:uid="{E2A4D83C-B912-7B40-B4E8-16962C46FDCD}"/>
+    <hyperlink ref="F7" r:id="rId28" xr:uid="{5CDB77A7-AAF0-FC42-AF10-BFF2A51455B2}"/>
+    <hyperlink ref="G7" r:id="rId29" xr:uid="{F85BEBCA-9721-9B4B-BA81-77D35B7DEAB2}"/>
+    <hyperlink ref="H7" r:id="rId30" xr:uid="{7694D138-B9E6-3549-8A2B-1EF40DCDF2B4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added functionality to handle .jpg links in addition to flickr pages.
</commit_message>
<xml_diff>
--- a/photolist.xlsx
+++ b/photolist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Aaron/Documents/Python Code/download_memorybook_photos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073A4750-9398-C549-9A7B-7554FFFA3948}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53795220-5055-5E48-A5F1-67ABED217316}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17660" yWindow="1140" windowWidth="17340" windowHeight="9580" xr2:uid="{9F72C116-6C8E-0D4A-8BDB-7E4359E9C28C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Team</t>
   </si>
@@ -69,6 +69,9 @@
     <t>Photo10</t>
   </si>
   <si>
+    <t>Drew Barklay</t>
+  </si>
+  <si>
     <t>https://www.flickr.com/photos/aaronhatcher/44303421911/in/album-72157699031593671/</t>
   </si>
   <si>
@@ -84,6 +87,9 @@
     <t>https://www.flickr.com/photos/aaronhatcher/29623981907/in/album-72157673213389378/</t>
   </si>
   <si>
+    <t>Ryan Gustafson</t>
+  </si>
+  <si>
     <t>https://www.flickr.com/photos/aaronhatcher/44815854251/in/album-72157695718027700/</t>
   </si>
   <si>
@@ -99,6 +105,9 @@
     <t>https://www.flickr.com/photos/aaronhatcher/29566593047/in/album-72157701022169035/</t>
   </si>
   <si>
+    <t>Alex Shaffer</t>
+  </si>
+  <si>
     <t>https://www.flickr.com/photos/aaronhatcher/42797091140/in/album-72157673289806428/</t>
   </si>
   <si>
@@ -114,6 +123,9 @@
     <t>https://www.flickr.com/photos/aaronhatcher/43004908230/in/album-72157695718027700/</t>
   </si>
   <si>
+    <t>Augie Phelps</t>
+  </si>
+  <si>
     <t>https://www.flickr.com/photos/aaronhatcher/44201224464/in/album-72157698526626812/</t>
   </si>
   <si>
@@ -129,6 +141,9 @@
     <t>https://www.flickr.com/photos/aaronhatcher/43397224615/in/album-72157699031593671/</t>
   </si>
   <si>
+    <t>Marcus Berger</t>
+  </si>
+  <si>
     <t>https://farm2.staticflickr.com/1978/44346511884_7b1fff907b_o_d.jpg</t>
   </si>
   <si>
@@ -142,6 +157,9 @@
   </si>
   <si>
     <t>https://farm2.staticflickr.com/1871/30634437668_9603c4f8b5_o_d.jpg</t>
+  </si>
+  <si>
+    <t>Jack Stonis</t>
   </si>
   <si>
     <t>https://www.flickr.com/photos/aaronhatcher/44666344741/in/album-72157673392276678/</t>
@@ -543,7 +561,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,26 +618,26 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="3">
         <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I2" s="3"/>
     </row>
@@ -627,26 +645,26 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
-        <v>2</v>
+      <c r="B3" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C3" s="3">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -654,26 +672,26 @@
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
-        <v>3</v>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C4" s="3">
         <v>16</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I4" s="3"/>
     </row>
@@ -681,26 +699,26 @@
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="3">
-        <v>4</v>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C5" s="3">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="I5" s="3"/>
     </row>
@@ -708,52 +726,52 @@
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>5</v>
+      <c r="B6" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C6" s="2">
         <v>17</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4">
-        <v>6</v>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="C7" s="4">
         <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>